<commit_message>
More work on JPADCore_v2 concerning ACAnalysisManager. New test in JPADSandBox_v2 in order to test a complete aircraft analysis (only weights and balance at the moment). Classpaths updated to the latest version of the Java jdk and jre (1.8.0_101).
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -225,7 +225,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.279112112054334</v>
+        <v>5.443642818356839</v>
       </c>
     </row>
     <row r="3">
@@ -236,7 +236,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.339062418656745</v>
+        <v>12.717880509399059</v>
       </c>
     </row>
     <row r="4">
@@ -247,7 +247,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>4.369154952029918</v>
+        <v>4.271532611314539</v>
       </c>
     </row>
     <row r="5">
@@ -258,7 +258,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>10.243962714994325</v>
+        <v>10.019195499471632</v>
       </c>
     </row>
     <row r="6">
@@ -269,7 +269,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>4.713011270971655</v>
+        <v>4.670094009256409</v>
       </c>
     </row>
     <row r="7">
@@ -280,7 +280,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.035662921955662</v>
+        <v>10.93684954232447</v>
       </c>
     </row>
     <row r="8">
@@ -291,7 +291,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>4.805473786353797</v>
+        <v>4.164794848457012</v>
       </c>
     </row>
     <row r="9">
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>11.248550074326452</v>
+        <v>9.773440792374878</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Update the jre to the version 1.8.0_111. Minor fix in MyChartToFileUtils.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -9,17 +9,18 @@
     <sheet name="GLOBAL RESULTS" r:id="rId3" sheetId="1"/>
     <sheet name="FUSELAGE" r:id="rId4" sheetId="2"/>
     <sheet name="WING" r:id="rId5" sheetId="3"/>
-    <sheet name="HORIZONTAL TAIL" r:id="rId6" sheetId="4"/>
-    <sheet name="VERTICAL TAIL" r:id="rId7" sheetId="5"/>
-    <sheet name="NACELLES" r:id="rId8" sheetId="6"/>
-    <sheet name="POWER PLANT" r:id="rId9" sheetId="7"/>
-    <sheet name="LANDING GEARS" r:id="rId10" sheetId="8"/>
+    <sheet name="FUEL TANK" r:id="rId6" sheetId="4"/>
+    <sheet name="HORIZONTAL TAIL" r:id="rId7" sheetId="5"/>
+    <sheet name="VERTICAL TAIL" r:id="rId8" sheetId="6"/>
+    <sheet name="NACELLES" r:id="rId9" sheetId="7"/>
+    <sheet name="POWER PLANT" r:id="rId10" sheetId="8"/>
+    <sheet name="LANDING GEARS" r:id="rId11" sheetId="9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -33,46 +34,55 @@
     <t>Xcg structure MAC</t>
   </si>
   <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Xcg structure BRF</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Zcg structure BRF</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Xcg structure BRF</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Xcg structure and engines MAC</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Xcg structure and engines BRF</t>
   </si>
   <si>
+    <t>Zcg structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Xcg operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>Xcg operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg operating empty mass BRF</t>
+  </si>
+  <si>
     <t>Xcg maximum zero fuel mass MAC</t>
   </si>
   <si>
     <t>Xcg maximum zero fuel mass BRF</t>
   </si>
   <si>
+    <t>Zcg maximum zero fuel mass BRF</t>
+  </si>
+  <si>
     <t>Xcg maximum take-off mass MAC</t>
   </si>
   <si>
     <t>Xcg maximum take-off mass BRF</t>
   </si>
   <si>
-    <t>Xcg operating empty mass (max aft)</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass (mean)</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass (max for)</t>
-  </si>
-  <si>
-    <t>Percent Error</t>
+    <t>Zcg maximum take-off mass BRF</t>
   </si>
   <si>
     <t>Xcg LRF</t>
@@ -102,25 +112,19 @@
     <t>TORENBEEK_1982</t>
   </si>
   <si>
+    <t>Ycg LRF (semi-wing)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (semi-wing)</t>
+  </si>
+  <si>
     <t>Ycg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
-    <t>Total Xcg LRF</t>
-  </si>
-  <si>
-    <t>Total Xcg BRF</t>
-  </si>
-  <si>
-    <t>Total Ycg LRF</t>
-  </si>
-  <si>
-    <t>Total Ycg BRF</t>
-  </si>
-  <si>
-    <t>Total Zcg LRF</t>
-  </si>
-  <si>
-    <t>Total Zcg BRF</t>
+    <t>Ycg LRF (semi-tail)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (semi-tail)</t>
   </si>
   <si>
     <t>BALANCE ESTIMATION FOR EACH NACELLE</t>
@@ -225,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.443642818356839</v>
+        <v>5.358157033106666</v>
       </c>
     </row>
     <row r="3">
@@ -236,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.717880509399059</v>
+        <v>12.521056690418195</v>
       </c>
     </row>
     <row r="4">
@@ -244,98 +248,167 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>4.271532611314539</v>
+        <v>0.7221121739534344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10.019195499471632</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>4.670094009256409</v>
+        <v>5.103819398632732</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>10.93684954232447</v>
+        <v>11.935465713143788</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>4.164794848457012</v>
+        <v>0.784349506445851</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="n">
-        <v>9.773440792374878</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>10.418043545381188</v>
+        <v>5.103819398632732</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.575603939312431</v>
+        <v>11.935465713143788</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.784349506445851</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.125710773137314</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>12.733164333243675</v>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>11.985868758750996</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.4871321042486384</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5.099577445159801</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="n">
+        <v>11.925698972626193</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.7143954860380879</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -361,13 +434,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -378,7 +448,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -389,7 +459,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -400,29 +470,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10.669199572303402</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>10.669199572303402</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -433,40 +497,45 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>10.74365914460681</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-12.115150927165407</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
+        <v>10.74365914460681</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
         <v>10.594739999999998</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-12.115150927165407</v>
       </c>
     </row>
   </sheetData>
@@ -492,13 +561,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -509,7 +575,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -520,7 +586,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -531,111 +597,104 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>12.21689315057678</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>4.735499999999997</v>
+        <v>12.21689315057678</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.5999999999999999</v>
+        <v>4.735499999999997</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.5999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-0.1313381437235337</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-112.74682089012906</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.216893150576782</v>
-      </c>
-      <c r="D11" t="n">
-        <v>18.103687116811845</v>
+        <v>-0.13133814372353347</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.216893150576782</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>20.71853476770793</v>
-      </c>
-      <c r="D14" t="n">
-        <v>282.82584567087844</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
+        <v>20.71853476770793</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
         <v>4.735499999999998</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-12.499999999999986</v>
       </c>
     </row>
   </sheetData>
@@ -661,35 +720,32 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6614514102920652</v>
+        <v>1.0771659522222063</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.3888239999999996</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -700,83 +756,45 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>25.961451410292064</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.3888239999999994</v>
+        <v>12.077165952222204</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>5.737399999999999</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.5999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.6614514102920652</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-19.098408721616277</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.3888239999999996</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-5.000000000000004</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -802,35 +820,32 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>0.6614514340216029</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9158</v>
+        <v>1.3888239999999996</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -841,83 +856,82 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>21.599999999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9157999999999998</v>
+        <v>25.9614514340216</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.2999999999999998</v>
+        <v>1.3888239999999994</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.737399999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2.111535413205652</v>
-      </c>
-      <c r="D10" t="n">
-        <v>33.64148184845897</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.6614514340216029</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9158</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-5.000000000000003</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.3888239999999996</v>
       </c>
     </row>
   </sheetData>
@@ -946,29 +960,29 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>2.5640710746536346</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.8316</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -979,29 +993,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>24.16407107465363</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1012,169 +1020,55 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.8315999999999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.5640710746536346</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.7483999999999997</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>10.317419999999998</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>4.573799999999999</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1.0289499999999998</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1.7483999999999997</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="n">
-        <v>10.317419999999998</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-4.573799999999999</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1.0289499999999998</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>4</v>
+        <v>1.8316</v>
       </c>
     </row>
   </sheetData>
@@ -1203,51 +1097,33 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>1.7483999999999997</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1258,7 +1134,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1269,82 +1145,76 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10.317419999999998</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.573799999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.0289499999999998</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.0649999999999995</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.0649999999999995</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>1.7483999999999997</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1355,83 +1225,66 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0649999999999995</v>
+        <v>10.317419999999998</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0649999999999995</v>
+        <v>-4.573799999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0</v>
+        <v>1.0289499999999998</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1460,51 +1313,33 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>12.499999999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>1.0649999999999995</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1522,6 +1357,212 @@
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.634019999999998</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.573799999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.0289499999999998</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.0649999999999995</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9.634019999999998</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-4.573799999999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.0289499999999998</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="25"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12.308548373872053</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.674638699878493</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning ACAnalysisManager in oreder to perform each analysis in a standalone mode. More work on JPADCore_v2 concerning take-off and landing analyses.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.358157033106666</v>
+        <v>5.355860654586927</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.521056690418195</v>
+        <v>12.515769472329737</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7221121739534344</v>
+        <v>0.71727723562519</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.103819398632732</v>
+        <v>5.1037246413394355</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.935465713143788</v>
+        <v>11.93524754245859</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.784349506445851</v>
+        <v>0.7800630108636133</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.103819398632732</v>
+        <v>5.1037246413394355</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.935465713143788</v>
+        <v>11.93524754245859</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.784349506445851</v>
+        <v>0.7800630108636133</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.125710773137314</v>
+        <v>5.125586989515182</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.985868758750996</v>
+        <v>11.985583757388909</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4871321042486384</v>
+        <v>0.4852401380055412</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>5.099577445159801</v>
+        <v>4.996891886241873</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.925698972626193</v>
+        <v>11.689274123731561</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7143954860380879</v>
+        <v>0.6983230019500191</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.308548373872053</v>
+        <v>12.302307460780472</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the Payload-Range analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.355860654586927</v>
+        <v>5.329030371724636</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.515769472329737</v>
+        <v>12.453995006296132</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.71727723562519</v>
+        <v>0.704518060315964</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.1037246413394355</v>
+        <v>5.090243222753136</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.93524754245859</v>
+        <v>11.904207711875411</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7800630108636133</v>
+        <v>0.7677698827414503</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.1037246413394355</v>
+        <v>5.090243222753136</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.93524754245859</v>
+        <v>11.904207711875411</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7800630108636133</v>
+        <v>0.7677698827414503</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.125586989515182</v>
+        <v>5.116284719535766</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.985583757388909</v>
+        <v>11.964166064410108</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4852401380055412</v>
+        <v>0.48122601702747003</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>4.996891886241873</v>
+        <v>4.992295568767794</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.689274123731561</v>
+        <v>11.67869148995392</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6983230019500191</v>
+        <v>0.6933403021326805</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.302307460780472</v>
+        <v>12.30269623209934</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning climb performance and operating conditions.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.329030371724636</v>
+        <v>5.358157033106666</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.453995006296132</v>
+        <v>12.521056690418195</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.704518060315964</v>
+        <v>0.7221121739534344</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.090243222753136</v>
+        <v>5.103819398632732</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.904207711875411</v>
+        <v>11.935465713143788</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7677698827414503</v>
+        <v>0.784349506445851</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.090243222753136</v>
+        <v>5.103819398632732</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.904207711875411</v>
+        <v>11.935465713143788</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7677698827414503</v>
+        <v>0.784349506445851</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.116284719535766</v>
+        <v>5.125710773137314</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.964166064410108</v>
+        <v>11.985868758750996</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.48122601702747003</v>
+        <v>0.4871321042486384</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>4.992295568767794</v>
+        <v>5.099577445159801</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.67869148995392</v>
+        <v>11.925698972626193</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6933403021326805</v>
+        <v>0.7143954860380879</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.30269623209934</v>
+        <v>12.308548373872053</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the performance analysis. Assigned polar curve can now be used for analyses.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.358157033106666</v>
+        <v>5.236520021021633</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.521056690418195</v>
+        <v>12.240997717128838</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7221121739534344</v>
+        <v>0.6576665053638682</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.103819398632732</v>
+        <v>5.041226939529571</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.935465713143788</v>
+        <v>11.791351849019662</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.784349506445851</v>
+        <v>0.721704678058392</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.103819398632732</v>
+        <v>5.041226939529571</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.935465713143788</v>
+        <v>11.791351849019662</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.784349506445851</v>
+        <v>0.721704678058392</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.125710773137314</v>
+        <v>5.081355335965858</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.985868758750996</v>
+        <v>11.883744101287732</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4871321042486384</v>
+        <v>0.46534746772689106</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>5.099577445159801</v>
+        <v>4.974961100839947</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.925698972626193</v>
+        <v>11.638780337853301</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7143954860380879</v>
+        <v>0.6736251083832776</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.308548373872053</v>
+        <v>12.299024241711926</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
New Matlab script added in DOCS in order to build a .h5 database of a given engine deck.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.236520021021633</v>
+        <v>5.219841746182212</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.240997717128838</v>
+        <v>12.202597394334816</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6576665053638682</v>
+        <v>0.6515745358190308</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.041226939529571</v>
+        <v>5.030926638536917</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.791351849019662</v>
+        <v>11.767636273709758</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.721704678058392</v>
+        <v>0.7154790360916665</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.041226939529571</v>
+        <v>5.030926638536917</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.791351849019662</v>
+        <v>11.767636273709758</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.721704678058392</v>
+        <v>0.7154790360916665</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.081355335965858</v>
+        <v>5.073941390864349</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.883744101287732</v>
+        <v>11.866674117262637</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.46534746772689106</v>
+        <v>0.4632885255976896</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>4.974961100839947</v>
+        <v>5.064594300942521</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.638780337853301</v>
+        <v>11.845153230142188</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6736251083832776</v>
+        <v>0.6833463972097202</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.299024241711926</v>
+        <v>12.298109362990228</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the balance analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.219841746182212</v>
+        <v>45.89293685237998</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.202597394334816</v>
+        <v>12.240997717128838</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6515745358190308</v>
+        <v>0.6576665053638682</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.030926638536917</v>
+        <v>26.36362870317379</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.767636273709758</v>
+        <v>11.791351849019662</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7154790360916665</v>
+        <v>0.721704678058392</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5.030926638536917</v>
+        <v>26.36362870317379</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.767636273709758</v>
+        <v>11.791351849019662</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7154790360916665</v>
+        <v>0.721704678058392</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>5.073941390864349</v>
+        <v>30.376468346802522</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.866674117262637</v>
+        <v>11.883744101287732</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4632885255976896</v>
+        <v>0.46534746772689106</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>5.064594300942521</v>
+        <v>19.737044834211375</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.845153230142188</v>
+        <v>11.638780337853301</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6833463972097202</v>
+        <v>0.6736251083832776</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.298109362990228</v>
+        <v>12.299024241711926</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the balance analysis. Max aft and fwd center of gravity calculation have been added. More work on the turboprop engine database MATLAB script.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Zcg maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Max aft Xcg MAC</t>
+  </si>
+  <si>
+    <t>Max forward Xcg MAC</t>
   </si>
   <si>
     <t>Xcg LRF</t>
@@ -411,6 +417,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="n">
+        <v>12.318389254421769</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>42.87685706504634</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -437,7 +465,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -448,7 +476,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -459,7 +487,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -475,7 +503,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -486,7 +514,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -497,7 +525,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -513,12 +541,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -529,7 +557,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -564,7 +592,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -575,7 +603,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -586,7 +614,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -602,7 +630,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -613,7 +641,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -624,7 +652,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -640,12 +668,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -656,7 +684,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -672,12 +700,12 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -688,7 +716,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -723,7 +751,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -734,7 +762,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -745,7 +773,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -761,7 +789,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -772,7 +800,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -783,7 +811,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -823,7 +851,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -834,7 +862,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -845,7 +873,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -861,7 +889,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -872,7 +900,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -883,7 +911,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -899,12 +927,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -920,12 +948,12 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -960,7 +988,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -971,7 +999,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -982,7 +1010,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -998,7 +1026,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1009,7 +1037,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1020,7 +1048,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1036,12 +1064,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1057,12 +1085,12 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1097,7 +1125,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -1107,12 +1135,12 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1123,7 +1151,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1134,7 +1162,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1150,7 +1178,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1161,7 +1189,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1172,7 +1200,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1198,12 +1226,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1214,7 +1242,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1225,7 +1253,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1241,7 +1269,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1252,7 +1280,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1263,7 +1291,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1313,7 +1341,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -1323,12 +1351,12 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1339,7 +1367,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1350,7 +1378,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1366,7 +1394,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1377,7 +1405,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1388,7 +1416,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1414,12 +1442,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1430,7 +1458,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1441,7 +1469,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1457,7 +1485,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1468,7 +1496,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1479,7 +1507,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1529,7 +1557,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1540,7 +1568,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1551,7 +1579,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Some errors have been fixed in the weights and balance analyses.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -235,7 +235,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>45.89293685237998</v>
+        <v>45.98540759259373</v>
       </c>
     </row>
     <row r="3">
@@ -246,7 +246,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.240997717128838</v>
+        <v>12.243126778022365</v>
       </c>
     </row>
     <row r="4">
@@ -257,7 +257,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6576665053638682</v>
+        <v>0.7144207146200321</v>
       </c>
     </row>
     <row r="5">
@@ -273,7 +273,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>26.36362870317379</v>
+        <v>26.286923460279134</v>
       </c>
     </row>
     <row r="7">
@@ -284,7 +284,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.791351849019662</v>
+        <v>11.789585775420619</v>
       </c>
     </row>
     <row r="8">
@@ -295,7 +295,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.721704678058392</v>
+        <v>0.7690953368472477</v>
       </c>
     </row>
     <row r="9">
@@ -311,7 +311,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>26.36362870317379</v>
+        <v>26.286923460279134</v>
       </c>
     </row>
     <row r="11">
@@ -322,7 +322,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.791351849019662</v>
+        <v>11.789585775420619</v>
       </c>
     </row>
     <row r="12">
@@ -333,7 +333,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.721704678058392</v>
+        <v>0.7690953368472477</v>
       </c>
     </row>
     <row r="13">
@@ -349,7 +349,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>30.376468346802522</v>
+        <v>30.337908673064945</v>
       </c>
     </row>
     <row r="15">
@@ -360,7 +360,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.883744101287732</v>
+        <v>11.882856297283656</v>
       </c>
     </row>
     <row r="16">
@@ -371,7 +371,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.46534746772689106</v>
+        <v>0.4950125969433359</v>
       </c>
     </row>
     <row r="17">
@@ -387,7 +387,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>19.737044834211375</v>
+        <v>32.013360757965835</v>
       </c>
     </row>
     <row r="19">
@@ -398,7 +398,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.638780337853301</v>
+        <v>11.921432170091581</v>
       </c>
     </row>
     <row r="20">
@@ -409,7 +409,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6736251083832776</v>
+        <v>0.7143833406573219</v>
       </c>
     </row>
     <row r="21">
@@ -425,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>12.318389254421769</v>
+        <v>12.193982195394145</v>
       </c>
     </row>
     <row r="23">
@@ -436,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>42.87685706504634</v>
+        <v>42.87406608391055</v>
       </c>
     </row>
   </sheetData>
@@ -673,55 +673,33 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.13133814372353347</v>
+        <v>1.216893150576782</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.216893150576782</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>20.71853476770793</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
         <v>4.735499999999998</v>
       </c>
     </row>
@@ -1054,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>1.8315999999999997</v>
+        <v>3.1315999999999997</v>
       </c>
     </row>
     <row r="9">
@@ -1563,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.299024241711926</v>
+        <v>12.297720537759226</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work JPADCore_v2 concerning the VMC calculation.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -85,10 +85,10 @@
     <t>Zcg maximum take-off mass BRF</t>
   </si>
   <si>
+    <t>Max forward Xcg MAC</t>
+  </si>
+  <si>
     <t>Max aft Xcg MAC</t>
-  </si>
-  <si>
-    <t>Max forward Xcg MAC</t>
   </si>
   <si>
     <t>Xcg LRF</t>

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the Aircraft class. More tests on JAXB
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -235,7 +235,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>45.98540759259373</v>
+        <v>45.985753259480774</v>
       </c>
     </row>
     <row r="3">
@@ -246,7 +246,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.243126778022365</v>
+        <v>12.2431106102261</v>
       </c>
     </row>
     <row r="4">
@@ -257,7 +257,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7144207146200321</v>
+        <v>0.7144023295588933</v>
       </c>
     </row>
     <row r="5">
@@ -273,7 +273,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>26.286923460279134</v>
+        <v>26.285360166326022</v>
       </c>
     </row>
     <row r="7">
@@ -284,7 +284,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>11.789585775420619</v>
+        <v>11.789564639151351</v>
       </c>
     </row>
     <row r="8">
@@ -295,7 +295,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7690953368472477</v>
+        <v>0.7690810854749826</v>
       </c>
     </row>
     <row r="9">
@@ -311,7 +311,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>26.286923460279134</v>
+        <v>26.285360166326022</v>
       </c>
     </row>
     <row r="11">
@@ -322,7 +322,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>11.789585775420619</v>
+        <v>11.789564639151351</v>
       </c>
     </row>
     <row r="12">
@@ -333,7 +333,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7690953368472477</v>
+        <v>0.7690810854749826</v>
       </c>
     </row>
     <row r="13">
@@ -349,7 +349,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>30.337908673064945</v>
+        <v>30.337014204087875</v>
       </c>
     </row>
     <row r="15">
@@ -360,7 +360,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.882856297283656</v>
+        <v>11.882842542608724</v>
       </c>
     </row>
     <row r="16">
@@ -371,7 +371,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4950125969433359</v>
+        <v>0.4950014667885061</v>
       </c>
     </row>
     <row r="17">
@@ -387,7 +387,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>32.013360757965835</v>
+        <v>31.95555501272207</v>
       </c>
     </row>
     <row r="19">
@@ -398,7 +398,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>11.921432170091581</v>
+        <v>11.920104878406033</v>
       </c>
     </row>
     <row r="20">
@@ -409,7 +409,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7143833406573219</v>
+        <v>0.7143756759170132</v>
       </c>
     </row>
     <row r="21">
@@ -425,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>12.193982195394145</v>
+        <v>12.191347548119742</v>
       </c>
     </row>
     <row r="23">
@@ -436,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>42.87406608391055</v>
+        <v>42.873991989932094</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +598,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.216893150576782</v>
+        <v>1.2168674857256812</v>
       </c>
     </row>
     <row r="3">
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>4.735499999999998</v>
+        <v>4.735499928277674</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.21689315057678</v>
+        <v>12.216867485725679</v>
       </c>
     </row>
     <row r="7">
@@ -647,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>4.735499999999997</v>
+        <v>4.735499928277673</v>
       </c>
     </row>
     <row r="8">
@@ -679,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.216893150576782</v>
+        <v>1.2168674857256812</v>
       </c>
     </row>
     <row r="12">
@@ -700,7 +700,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>4.735499999999998</v>
+        <v>4.735499928277674</v>
       </c>
     </row>
   </sheetData>
@@ -735,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0771659522222063</v>
+        <v>1.0705347356137023</v>
       </c>
     </row>
     <row r="3">
@@ -773,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.077165952222204</v>
+        <v>12.0705347356137</v>
       </c>
     </row>
     <row r="7">
@@ -1541,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.297720537759226</v>
+        <v>12.297653141047952</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Review of weights, balance and performance modules: tests on ATR-72 model.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -43,6 +43,9 @@
     <t>m</t>
   </si>
   <si>
+    <t>Zcg structure MAC</t>
+  </si>
+  <si>
     <t>Zcg structure BRF</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>Xcg structure and engines BRF</t>
   </si>
   <si>
+    <t>Zcg structure and engines MAC</t>
+  </si>
+  <si>
     <t>Zcg structure and engines BRF</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t>Xcg operating empty mass BRF</t>
   </si>
   <si>
+    <t>Zcg operating empty mass MAC</t>
+  </si>
+  <si>
     <t>Zcg operating empty mass BRF</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t>Xcg maximum zero fuel mass BRF</t>
   </si>
   <si>
+    <t>Zcg maximum zero fuel mass MAC</t>
+  </si>
+  <si>
     <t>Zcg maximum zero fuel mass BRF</t>
   </si>
   <si>
@@ -80,6 +92,9 @@
   </si>
   <si>
     <t>Xcg maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg maximum take-off mass MAC</t>
   </si>
   <si>
     <t>Zcg maximum take-off mass BRF</t>
@@ -235,7 +250,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>45.985753259480774</v>
+        <v>54.44126671372609</v>
       </c>
     </row>
     <row r="3">
@@ -246,7 +261,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.2431106102261</v>
+        <v>12.437815810838156</v>
       </c>
     </row>
     <row r="4">
@@ -254,26 +269,26 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7144023295588933</v>
+        <v>27.67850347037711</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.637274225272874</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="n">
-        <v>26.285360166326022</v>
       </c>
     </row>
     <row r="7">
@@ -281,10 +296,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>11.789564639151351</v>
+        <v>32.206395870082275</v>
       </c>
     </row>
     <row r="8">
@@ -295,34 +310,34 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7690810854749826</v>
+        <v>11.925876640929975</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30.784599937879275</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>26.285360166326022</v>
+        <v>0.708789479776021</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11.789564639151351</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -330,113 +345,168 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7690810854749826</v>
+        <v>32.206395870082275</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11.925876640929975</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>30.337014204087875</v>
+        <v>30.784599937879275</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>11.882842542608724</v>
+        <v>0.708789479776021</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.4950014667885061</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>34.28982845054642</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>31.95555501272207</v>
+        <v>11.973845920954258</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>11.920104878406033</v>
+        <v>20.6733270276342</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7143756759170132</v>
+        <v>0.4759859390320157</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>12.191347548119742</v>
+        <v>54.284755273589916</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12.434212266778562</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="n">
-        <v>42.873991989932094</v>
+      <c r="C24" t="n">
+        <v>27.842825670894356</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.6410576055102428</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>18.282686812078495</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="n">
+        <v>54.284755273589916</v>
       </c>
     </row>
   </sheetData>
@@ -465,18 +535,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>10.669199572303402</v>
+        <v>11.04753745546374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -487,7 +557,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -498,23 +568,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>10.669199572303402</v>
+        <v>11.04753745546374</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -525,7 +595,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -536,28 +606,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>10.74365914460681</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -592,29 +662,29 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.2168674857256812</v>
+        <v>1.330689739372911</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>4.735499928277674</v>
+        <v>4.735499999999998</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -625,34 +695,34 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.216867485725679</v>
+        <v>12.33068973937291</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>4.735499928277673</v>
+        <v>4.735499999999997</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -663,44 +733,44 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.2168674857256812</v>
+        <v>1.330689739372911</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>4.735499928277674</v>
+        <v>4.735499999999998</v>
       </c>
     </row>
   </sheetData>
@@ -729,18 +799,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0705347356137023</v>
+        <v>1.0717832283332958</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -751,7 +821,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -762,23 +832,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.0705347356137</v>
+        <v>12.071783228333294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -789,7 +859,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -800,7 +870,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -829,18 +899,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6614514340216029</v>
+        <v>0.7599657170108016</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -851,7 +921,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -862,23 +932,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>25.9614514340216</v>
+        <v>26.059965717010797</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -889,7 +959,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -900,38 +970,38 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6614514340216029</v>
+        <v>0.7599657170108016</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -966,18 +1036,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.5640710746536337</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -988,7 +1058,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -999,12 +1069,12 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1015,7 +1085,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1026,7 +1096,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1037,38 +1107,38 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.5640710746536337</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1103,22 +1173,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1129,7 +1199,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1140,7 +1210,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1151,12 +1221,12 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1167,7 +1237,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1178,7 +1248,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1189,27 +1259,27 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1220,7 +1290,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1231,7 +1301,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1242,12 +1312,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1258,7 +1328,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1269,7 +1339,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1280,17 +1350,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1319,22 +1389,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1345,7 +1415,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1356,7 +1426,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1367,12 +1437,12 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1383,7 +1453,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1394,7 +1464,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1405,27 +1475,27 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1436,7 +1506,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1447,7 +1517,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1458,12 +1528,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1474,7 +1544,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1485,7 +1555,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1496,17 +1566,17 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1535,18 +1605,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.297653141047952</v>
+        <v>12.321708214766055</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1557,18 +1627,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.674638699878493</v>
+        <v>-1.8746386998784927</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ACPerformanceManager: Completed. More work on ACAnalysisManager and ACBalanceManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -254,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>54.590553373497784</v>
+        <v>60.540708391007826</v>
       </c>
     </row>
     <row r="3">
@@ -265,7 +265,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.441253010416212</v>
+        <v>12.578250317120148</v>
       </c>
     </row>
     <row r="4">
@@ -276,7 +276,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>27.67850347037711</v>
+        <v>24.183035275777005</v>
       </c>
     </row>
     <row r="5">
@@ -287,7 +287,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.637274225272874</v>
+        <v>0.5567940147707489</v>
       </c>
     </row>
     <row r="6">
@@ -303,7 +303,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>32.328424593171725</v>
+        <v>43.608243744263845</v>
       </c>
     </row>
     <row r="8">
@@ -314,7 +314,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>11.928686249478758</v>
+        <v>12.188394583002776</v>
       </c>
     </row>
     <row r="9">
@@ -325,7 +325,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>30.784599937879275</v>
+        <v>26.8984357935812</v>
       </c>
     </row>
     <row r="10">
@@ -336,7 +336,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.708789479776021</v>
+        <v>0.6193138241651133</v>
       </c>
     </row>
     <row r="11">
@@ -352,7 +352,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>32.328424593171725</v>
+        <v>43.608243744263845</v>
       </c>
     </row>
     <row r="13">
@@ -363,7 +363,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>11.928686249478758</v>
+        <v>12.188394583002776</v>
       </c>
     </row>
     <row r="14">
@@ -374,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>30.784599937879275</v>
+        <v>26.8984357935812</v>
       </c>
     </row>
     <row r="15">
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>0.708789479776021</v>
+        <v>0.6193138241651133</v>
       </c>
     </row>
     <row r="16">
@@ -401,7 +401,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>34.37507043143105</v>
+        <v>42.16856219521241</v>
       </c>
     </row>
     <row r="18">
@@ -412,7 +412,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>11.975808545753935</v>
+        <v>12.155247128163197</v>
       </c>
     </row>
     <row r="19">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>20.6733270276342</v>
+        <v>17.525864882468294</v>
       </c>
     </row>
     <row r="20">
@@ -434,7 +434,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4759859390320157</v>
+        <v>0.40351827464824574</v>
       </c>
     </row>
     <row r="21">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>54.36201386653654</v>
+        <v>41.66724914526735</v>
       </c>
     </row>
     <row r="23">
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>12.435991080796395</v>
+        <v>12.143704817508112</v>
       </c>
     </row>
     <row r="24">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>27.842825670894356</v>
+        <v>24.712347950739662</v>
       </c>
     </row>
     <row r="25">
@@ -483,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6410576055102428</v>
+        <v>0.5689809932042091</v>
       </c>
     </row>
     <row r="26">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>18.393551812392595</v>
+        <v>29.55032474357941</v>
       </c>
     </row>
     <row r="28">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>54.36201386653654</v>
+        <v>56.77536475163592</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1647,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.321708214766055</v>
+        <v>12.321629305144317</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Write aircraft to file: Completed. More work on JPADCommander.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -254,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>60.540708391007826</v>
+        <v>60.58379194471799</v>
       </c>
     </row>
     <row r="3">
@@ -265,7 +265,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.578250317120148</v>
+        <v>12.578175260813666</v>
       </c>
     </row>
     <row r="4">
@@ -276,7 +276,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>24.183035275777005</v>
+        <v>24.22129792720768</v>
       </c>
     </row>
     <row r="5">
@@ -287,7 +287,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5567940147707489</v>
+        <v>0.5567252463403136</v>
       </c>
     </row>
     <row r="6">
@@ -303,7 +303,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>43.608243744263845</v>
+        <v>43.62176109828424</v>
       </c>
     </row>
     <row r="8">
@@ -314,7 +314,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>12.188394583002776</v>
+        <v>12.188303882748276</v>
       </c>
     </row>
     <row r="9">
@@ -325,7 +325,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>26.8984357935812</v>
+        <v>26.942174991215605</v>
       </c>
     </row>
     <row r="10">
@@ -336,7 +336,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6193138241651133</v>
+        <v>0.6192644611368907</v>
       </c>
     </row>
     <row r="11">
@@ -352,7 +352,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>43.608243744263845</v>
+        <v>43.62176109828424</v>
       </c>
     </row>
     <row r="13">
@@ -363,7 +363,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>12.188394583002776</v>
+        <v>12.188303882748276</v>
       </c>
     </row>
     <row r="14">
@@ -374,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>26.8984357935812</v>
+        <v>26.942174991215605</v>
       </c>
     </row>
     <row r="15">
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6193138241651133</v>
+        <v>0.6192644611368907</v>
       </c>
     </row>
     <row r="16">
@@ -401,7 +401,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>42.16856219521241</v>
+        <v>54.03205126990302</v>
       </c>
     </row>
     <row r="18">
@@ -412,7 +412,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>12.155247128163197</v>
+        <v>12.427583849399376</v>
       </c>
     </row>
     <row r="19">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>17.525864882468294</v>
+        <v>17.554146471108247</v>
       </c>
     </row>
     <row r="20">
@@ -434,7 +434,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.40351827464824574</v>
+        <v>0.4034811242482551</v>
       </c>
     </row>
     <row r="21">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>41.66724914526735</v>
+        <v>51.99537149805351</v>
       </c>
     </row>
     <row r="23">
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>12.143704817508112</v>
+        <v>12.380770873021856</v>
       </c>
     </row>
     <row r="24">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>24.712347950739662</v>
+        <v>24.75311268810642</v>
       </c>
     </row>
     <row r="25">
@@ -483,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5689809932042091</v>
+        <v>0.5689489803721794</v>
       </c>
     </row>
     <row r="26">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>29.55032474357941</v>
+        <v>29.539801660785603</v>
       </c>
     </row>
     <row r="28">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>56.77536475163592</v>
+        <v>66.10696498785293</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.330689739372911</v>
+        <v>1.3305081214942964</v>
       </c>
     </row>
     <row r="3">
@@ -718,7 +718,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.33068973937291</v>
+        <v>12.330508121494294</v>
       </c>
     </row>
     <row r="7">
@@ -761,7 +761,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.330689739372911</v>
+        <v>1.3305081214942964</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0717832283332958</v>
+        <v>1.089073330329886</v>
       </c>
     </row>
     <row r="3">
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>12.071783228333294</v>
+        <v>12.089073330329885</v>
       </c>
     </row>
     <row r="7">
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2.5640710746536337</v>
+        <v>2.5640710746536346</v>
       </c>
     </row>
     <row r="3">
@@ -1104,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>24.16407107465363</v>
+        <v>24.164071074653634</v>
       </c>
     </row>
     <row r="7">
@@ -1147,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2.5640710746536337</v>
+        <v>2.5640710746536346</v>
       </c>
     </row>
     <row r="12">
@@ -1260,7 +1260,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>10.317419999999998</v>
+        <v>10.3174</v>
       </c>
     </row>
     <row r="10">
@@ -1282,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0289499999999998</v>
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="12">
@@ -1351,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>10.317419999999998</v>
+        <v>10.3174</v>
       </c>
     </row>
     <row r="21">
@@ -1373,7 +1373,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0289499999999998</v>
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="23">
@@ -1480,7 +1480,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>9.634019999999998</v>
+        <v>9.633999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1502,7 +1502,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0289499999999998</v>
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="12">
@@ -1571,7 +1571,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>9.634019999999998</v>
+        <v>9.633999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1593,7 +1593,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0289499999999998</v>
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="23">
@@ -1647,7 +1647,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.321629305144317</v>
+        <v>12.321363937165607</v>
       </c>
     </row>
     <row r="3">
@@ -1669,7 +1669,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.8746386998784927</v>
+        <v>-1.874638699878493</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Debugging Aerodynamic and Stability
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -254,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>60.58379194471799</v>
+        <v>59.75763069502311</v>
       </c>
     </row>
     <row r="3">
@@ -265,7 +265,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.578175260813666</v>
+        <v>12.559185988371063</v>
       </c>
     </row>
     <row r="4">
@@ -276,7 +276,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>24.22129792720768</v>
+        <v>23.951837906491903</v>
       </c>
     </row>
     <row r="5">
@@ -287,7 +287,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5567252463403136</v>
+        <v>0.5505317220765564</v>
       </c>
     </row>
     <row r="6">
@@ -303,7 +303,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>43.62176109828424</v>
+        <v>43.12093038555306</v>
       </c>
     </row>
     <row r="8">
@@ -314,7 +314,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>12.188303882748276</v>
+        <v>12.17679231541782</v>
       </c>
     </row>
     <row r="9">
@@ -325,7 +325,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>26.942174991215605</v>
+        <v>26.673077984574366</v>
       </c>
     </row>
     <row r="10">
@@ -336,7 +336,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6192644611368907</v>
+        <v>0.6130792807323548</v>
       </c>
     </row>
     <row r="11">
@@ -352,7 +352,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>43.62176109828424</v>
+        <v>43.12093038555306</v>
       </c>
     </row>
     <row r="13">
@@ -363,7 +363,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>12.188303882748276</v>
+        <v>12.17679231541782</v>
       </c>
     </row>
     <row r="14">
@@ -374,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>26.942174991215605</v>
+        <v>26.673077984574366</v>
       </c>
     </row>
     <row r="15">
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6192644611368907</v>
+        <v>0.6130792807323548</v>
       </c>
     </row>
     <row r="16">
@@ -401,7 +401,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>54.03205126990302</v>
+        <v>53.6519945733621</v>
       </c>
     </row>
     <row r="18">
@@ -412,7 +412,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>12.427583849399376</v>
+        <v>12.41884826641613</v>
       </c>
     </row>
     <row r="19">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>17.554146471108247</v>
+        <v>17.426005229321305</v>
       </c>
     </row>
     <row r="20">
@@ -434,7 +434,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4034811242482551</v>
+        <v>0.40053580461201665</v>
       </c>
     </row>
     <row r="21">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>51.99537149805351</v>
+        <v>51.66787324255058</v>
       </c>
     </row>
     <row r="23">
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>12.380770873021856</v>
+        <v>12.37324334301422</v>
       </c>
     </row>
     <row r="24">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>24.75311268810642</v>
+        <v>24.642692233671223</v>
       </c>
     </row>
     <row r="25">
@@ -483,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5689489803721794</v>
+        <v>0.5664109720919794</v>
       </c>
     </row>
     <row r="26">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>0.29539801660785603</v>
+        <v>0.29186955894857564</v>
       </c>
     </row>
     <row r="28">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6610696498785293</v>
+        <v>0.6562640112814851</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1647,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.321363937165607</v>
+        <v>12.318240617784834</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Fixed some errors in Aeordynamic and Stability
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -254,7 +254,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>59.75763069502311</v>
+        <v>59.73179055824007</v>
       </c>
     </row>
     <row r="3">
@@ -265,7 +265,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>12.559185988371063</v>
+        <v>12.558592054199604</v>
       </c>
     </row>
     <row r="4">
@@ -276,7 +276,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>23.951837906491903</v>
+        <v>23.881283765287307</v>
       </c>
     </row>
     <row r="5">
@@ -287,7 +287,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5505317220765564</v>
+        <v>0.5489100388884587</v>
       </c>
     </row>
     <row r="6">
@@ -303,7 +303,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>43.12093038555306</v>
+        <v>43.11606869451627</v>
       </c>
     </row>
     <row r="8">
@@ -314,7 +314,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>12.17679231541782</v>
+        <v>12.176680569707568</v>
       </c>
     </row>
     <row r="9">
@@ -325,7 +325,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>26.673077984574366</v>
+        <v>26.608857770674003</v>
       </c>
     </row>
     <row r="10">
@@ -336,7 +336,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6130792807323548</v>
+        <v>0.6116031825269179</v>
       </c>
     </row>
     <row r="11">
@@ -352,7 +352,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>43.12093038555306</v>
+        <v>43.11606869451627</v>
       </c>
     </row>
     <row r="13">
@@ -363,7 +363,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>12.17679231541782</v>
+        <v>12.176680569707568</v>
       </c>
     </row>
     <row r="14">
@@ -374,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>26.673077984574366</v>
+        <v>26.608857770674003</v>
       </c>
     </row>
     <row r="15">
@@ -385,7 +385,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6130792807323548</v>
+        <v>0.6116031825269179</v>
       </c>
     </row>
     <row r="16">
@@ -401,7 +401,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>53.6519945733621</v>
+        <v>53.60136223687021</v>
       </c>
     </row>
     <row r="18">
@@ -412,7 +412,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>12.41884826641613</v>
+        <v>12.417684484851204</v>
       </c>
     </row>
     <row r="19">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>17.426005229321305</v>
+        <v>17.425612078158753</v>
       </c>
     </row>
     <row r="20">
@@ -434,7 +434,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.40053580461201665</v>
+        <v>0.4005267680534276</v>
       </c>
     </row>
     <row r="21">
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>51.66787324255058</v>
+        <v>51.624242905224534</v>
       </c>
     </row>
     <row r="23">
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>12.37324334301422</v>
+        <v>12.372240502028212</v>
       </c>
     </row>
     <row r="24">
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>24.642692233671223</v>
+        <v>24.64235345179721</v>
       </c>
     </row>
     <row r="25">
@@ -483,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5664109720919794</v>
+        <v>0.5664031852085996</v>
       </c>
     </row>
     <row r="26">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>0.29186955894857564</v>
+        <v>0.29269052532561396</v>
       </c>
     </row>
     <row r="28">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6562640112814851</v>
+        <v>0.6551257388670622</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1647,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>12.318240617784834</v>
+        <v>12.32108109437063</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More tests on ATR72
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -15,12 +15,13 @@
     <sheet name="NACELLES" r:id="rId9" sheetId="7"/>
     <sheet name="POWER PLANT" r:id="rId10" sheetId="8"/>
     <sheet name="LANDING GEARS" r:id="rId11" sheetId="9"/>
+    <sheet name="SYSTEMS" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="73">
   <si>
     <t>Description</t>
   </si>
@@ -31,73 +32,139 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Xcg structure MAC</t>
+    <t>STRUCTURAL MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Structure BRF</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ycg Structure BRF</t>
+  </si>
+  <si>
+    <t>Zcg Structure BRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Xcg Structure MAC</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>Xcg structure BRF</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Zcg structure MAC</t>
-  </si>
-  <si>
-    <t>Zcg structure BRF</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Xcg structure and engines MAC</t>
-  </si>
-  <si>
-    <t>Xcg structure and engines BRF</t>
-  </si>
-  <si>
-    <t>Zcg structure and engines MAC</t>
-  </si>
-  <si>
-    <t>Zcg structure and engines BRF</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg operating empty mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg operating empty mass BRF</t>
-  </si>
-  <si>
-    <t>Xcg maximum zero fuel mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg maximum zero fuel mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg maximum zero fuel mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg maximum zero fuel mass BRF</t>
-  </si>
-  <si>
-    <t>Xcg maximum take-off mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg maximum take-off mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg maximum take-off mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg maximum take-off mass BRF</t>
+    <t>Ycg Structure MAC</t>
+  </si>
+  <si>
+    <t>Zcg Structure MAC</t>
+  </si>
+  <si>
+    <t>STRUCTURAL MASS PLUS POWER PLANT CG</t>
+  </si>
+  <si>
+    <t>Xcg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Ycg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Zcg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Xcg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>Ycg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>Zcg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>MANUFACTURER EMPTY MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>OPERATING EMPTY MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>MAXIMUM ZERO-FUEL MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>MAXIMUM TAKE-OFF MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Maximum take-off mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Maximum take-off mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Maximum take-off mass MAC</t>
   </si>
   <si>
     <t>Max forward Xcg MAC</t>
@@ -127,12 +194,12 @@
     <t>Xcg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
   </si>
   <si>
-    <t>TORENBEEK_1982</t>
-  </si>
-  <si>
     <t>Ycg LRF (semi-wing)</t>
   </si>
   <si>
@@ -148,22 +215,31 @@
     <t>Ycg BRF (semi-tail)</t>
   </si>
   <si>
-    <t>BALANCE ESTIMATION FOR EACH NACELLE</t>
-  </si>
-  <si>
-    <t>NACELLE 1</t>
-  </si>
-  <si>
-    <t>NACELLE 2</t>
-  </si>
-  <si>
-    <t>BALANCE ESTIMATION FOR EACH ENGINE</t>
-  </si>
-  <si>
-    <t>ENGINE 1</t>
-  </si>
-  <si>
-    <t>ENGINE 2</t>
+    <t>TORENBEEK_1976</t>
+  </si>
+  <si>
+    <t>Zcg ESTIMATION METHOD COMPARISON</t>
+  </si>
+  <si>
+    <t>APU</t>
+  </si>
+  <si>
+    <t>AIR CONDITIONING AND ANTI-ICING SYSTEM</t>
+  </si>
+  <si>
+    <t>INSTRUMENTS AND NAVIGATION SYSTEM</t>
+  </si>
+  <si>
+    <t>HYDRAULIC AND PNEUMATIC SYSTEMS</t>
+  </si>
+  <si>
+    <t>ELECTRICAL SYSTEMS</t>
+  </si>
+  <si>
+    <t>CONTROL SURFACES</t>
+  </si>
+  <si>
+    <t>FURNISHINGS AND EQUIPMENTS</t>
   </si>
 </sst>
 </file>
@@ -250,60 +326,54 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>59.73179055824007</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>12.558592054199604</v>
+        <v>12.383094664400438</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>23.881283765287307</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5489100388884587</v>
+        <v>0.5752016084174996</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>43.11606869451627</v>
+        <v>52.06458273450066</v>
       </c>
     </row>
     <row r="8">
@@ -311,10 +381,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>12.176680569707568</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -322,195 +392,801 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>26.608857770674003</v>
+        <v>24.98252570615605</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.6116031825269179</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="n">
-        <v>43.11606869451627</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>12.176680569707568</v>
+        <v>11.77864288751444</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>26.608857770674003</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6116031825269179</v>
+        <v>0.6726749619652885</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>53.60136223687021</v>
+        <v>25.811644924171027</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>12.417684484851204</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>17.425612078158753</v>
+        <v>29.216051004133615</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4005267680534276</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="n">
-        <v>51.624242905224534</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>12.372240502028212</v>
+        <v>11.261596322758468</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>24.64235345179721</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5664031852085996</v>
+        <v>0.8141395635175535</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>0.29269052532561396</v>
+        <v>3.354946427041492</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="n">
+        <v>35.36023244081936</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>11.261596322758468</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.8141395635175535</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3.354946427041492</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="n">
+        <v>35.36023244081936</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>11.659199385705143</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.5300954726368827</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="n">
+        <v>20.623898035573717</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="n">
+        <v>23.023447045467204</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>11.932509279597955</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.7489236603097895</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="n">
+        <v>32.494468892823456</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="n">
+        <v>32.52773344482285</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-10.89270205720054</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="n">
+        <v>33.15878000122252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22.47171519999999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11.643974999999998</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.032016799999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>15.024825313991244</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.9617727039715156</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>7.854004299999998</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.46857499999999996</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6551257388670622</v>
+        <v>10.015123773098278</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4.452521311514449</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>12.485493599999996</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.6628499999999999</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -543,10 +1219,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>11.04753745546374</v>
@@ -554,10 +1230,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -565,10 +1241,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -576,15 +1252,15 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>11.04753745546374</v>
@@ -592,10 +1268,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -603,10 +1279,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -614,34 +1290,34 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>11.500334910927485</v>
+        <v>10.594739999999998</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>10.594739999999998</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
   </sheetData>
@@ -674,32 +1350,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.3305081214942964</v>
+        <v>0.9501850770480618</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>4.735499999999998</v>
+        <v>5.411999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -707,37 +1383,37 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>12.330508121494294</v>
+        <v>11.95018507704806</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>4.735499999999997</v>
+        <v>5.411999999999998</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>1.5999999999999999</v>
@@ -745,44 +1421,66 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.3305081214942964</v>
+        <v>1.0876479268177373</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8127222272783863</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>4.735499999999998</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.411999999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13.175946919719877</v>
       </c>
     </row>
   </sheetData>
@@ -815,21 +1513,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.089073330329886</v>
+        <v>1.0717832283332958</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -837,10 +1535,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -848,26 +1546,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>12.089073330329885</v>
+        <v>12.071783228333294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -875,10 +1573,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>1.5999999999999999</v>
@@ -886,7 +1584,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -919,21 +1617,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8841681842937887</v>
+        <v>0.8841681842937885</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>1.3888239999999996</v>
@@ -941,10 +1639,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -952,15 +1650,15 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>26.184168184293785</v>
@@ -968,21 +1666,21 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.3888239999999994</v>
+        <v>1.3888239999999996</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>5.737399999999999</v>
@@ -990,44 +1688,44 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8841681842937887</v>
+        <v>0.8841681842937885</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>1.3888239999999996</v>
+        <v>1.3888239999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1060,32 +1758,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.9689712922618385</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>1.8316</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -1093,26 +1791,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>24.164071074653634</v>
+        <v>24.568971292261836</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -1120,55 +1818,55 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3.1315999999999997</v>
+        <v>1.2999999999999998</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>2.5640710746536346</v>
+        <v>2.9689712922618385</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>1.8316</v>
+        <v>2.651</v>
       </c>
     </row>
   </sheetData>
@@ -1201,194 +1899,94 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.7483999999999997</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>10.568999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>4.573799999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="n">
-        <v>10.3174</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.573799999999999</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0289999999999997</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.7483999999999997</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>10.3174</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-4.573799999999999</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1.0289999999999997</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>9</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -1421,194 +2019,94 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.0649999999999995</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>9.568999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>4.573799999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0289999999999997</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="n">
-        <v>9.633999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.573799999999999</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0289999999999997</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.0649999999999995</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9.633999999999999</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-4.573799999999999</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1.0289999999999997</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>9</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1641,21 +2139,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>12.32108109437063</v>
+        <v>10.465315107125335</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -1663,10 +2161,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>-1.874638699878493</v>
@@ -1674,7 +2172,82 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.465315107125335</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.874638699878493</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10.465315107125335</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-1.874638699878493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aerodynamic features testing in progress
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -382,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>12.126008124433021</v>
+        <v>12.493732778839664</v>
       </c>
     </row>
     <row r="4">
@@ -404,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.11681320524249036</v>
+        <v>0.2026367917785099</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>56.81731846831799</v>
+        <v>72.66591192694396</v>
       </c>
     </row>
     <row r="8">
@@ -442,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>5.034541411085246</v>
+        <v>8.73345883712879</v>
       </c>
     </row>
     <row r="10">
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>11.773059195085036</v>
+        <v>12.077002477595759</v>
       </c>
     </row>
     <row r="14">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2646154298484543</v>
+        <v>0.3344168742828306</v>
       </c>
     </row>
     <row r="16">
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>41.6055451323161</v>
+        <v>54.70522028672069</v>
       </c>
     </row>
     <row r="18">
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>11.404680976081776</v>
+        <v>14.41305885449827</v>
       </c>
     </row>
     <row r="20">
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>11.773059195085036</v>
+        <v>12.077002477595759</v>
       </c>
     </row>
     <row r="24">
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.2646154298484543</v>
+        <v>0.3344168742828306</v>
       </c>
     </row>
     <row r="26">
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>41.6055451323161</v>
+        <v>54.70522028672069</v>
       </c>
     </row>
     <row r="28">
@@ -614,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>11.404680976081776</v>
+        <v>14.41305885449827</v>
       </c>
     </row>
     <row r="30">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>11.773059195085036</v>
+        <v>12.077002477595759</v>
       </c>
     </row>
     <row r="34">
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>0.2646154298484543</v>
+        <v>0.3344168742828306</v>
       </c>
     </row>
     <row r="36">
@@ -678,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>41.6055451323161</v>
+        <v>54.70522028672069</v>
       </c>
     </row>
     <row r="38">
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>11.404680976081776</v>
+        <v>14.41305885449827</v>
       </c>
     </row>
     <row r="40">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>11.968154587348053</v>
+        <v>12.167174374084453</v>
       </c>
     </row>
     <row r="44">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1799825575054031</v>
+        <v>0.23196738512587894</v>
       </c>
     </row>
     <row r="46">
@@ -764,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>50.01397660563383</v>
+        <v>58.591545861350966</v>
       </c>
     </row>
     <row r="48">
@@ -786,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>7.757082233579379</v>
+        <v>9.997580359284555</v>
       </c>
     </row>
     <row r="50">
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>11.916579023490726</v>
+        <v>12.088275972424078</v>
       </c>
     </row>
     <row r="54">
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.4685790495763851</v>
+        <v>0.4703444584044726</v>
       </c>
     </row>
     <row r="56">
@@ -850,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>47.79111737066325</v>
+        <v>55.19109751646549</v>
       </c>
     </row>
     <row r="58">
@@ -872,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>20.195324874119375</v>
+        <v>20.271412366402902</v>
       </c>
     </row>
     <row r="60">
@@ -893,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>26.951502019811024</v>
+        <v>39.62465381505397</v>
       </c>
     </row>
     <row r="63">
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>47.79111737066325</v>
+        <v>55.19109751646549</v>
       </c>
     </row>
     <row r="64">
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>62.54519375869836</v>
+        <v>72.22238919493513</v>
       </c>
     </row>
     <row r="65">
@@ -946,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>47917.67515197389</v>
+        <v>48847.102313419484</v>
       </c>
     </row>
     <row r="70">
@@ -957,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>752384.2326572407</v>
+        <v>833511.1570649091</v>
       </c>
     </row>
     <row r="71">
@@ -968,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>704466.5575052667</v>
+        <v>784664.0547514894</v>
       </c>
     </row>
     <row r="72">
@@ -1011,7 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>47822.26916540071</v>
+        <v>56924.64455993669</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>10.594739999999998</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>11.500334910927485</v>
+        <v>10.594739999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>1.104420538817831</v>
+        <v>0.8545440651259495</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8545440651259495</v>
+        <v>1.104420538817831</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>5.409999999999998</v>
+        <v>10.998778735632179</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>10.998778735632179</v>
+        <v>5.409999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2837,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>-11.300829133796222</v>
+        <v>-11.461146791155318</v>
       </c>
     </row>
     <row r="6">
@@ -2848,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>-11.300829133796261</v>
+        <v>-11.461146791155358</v>
       </c>
     </row>
     <row r="7">
@@ -2859,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>10.545506842019538</v>
+        <v>10.54178709519774</v>
       </c>
     </row>
     <row r="8">
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>10.545506842019536</v>
+        <v>10.54178709519774</v>
       </c>
     </row>
     <row r="9">
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>10.545506842019536</v>
+        <v>10.54178709519774</v>
       </c>
     </row>
     <row r="10">
@@ -2892,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>10.545506842019535</v>
+        <v>10.54178709519774</v>
       </c>
     </row>
     <row r="11">
@@ -3005,13 +3005,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>10.545506842019538</v>
+        <v>10.54178709519774</v>
       </c>
     </row>
     <row r="24">
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>